<commit_message>
MOD: requisitos, documentação e ppt
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Requisitos/Requisitos.xlsx
+++ b/Documentação/Planilha de Requisitos/Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\Documentação\Planilha de Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fecco\OneDrive\Documentos\project-hunter\Documentação\Planilha de Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9333F3B-971C-4803-A8B2-8F3B51C1B17B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD912B0-C3BA-459E-A7F6-EAD0089A534D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6C75A49A-3A66-4F18-864E-6536A5F66FE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6C75A49A-3A66-4F18-864E-6536A5F66FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>O softaware deve conter uma tela de login</t>
   </si>
@@ -154,6 +154,90 @@
   </si>
   <si>
     <t>O projeto deve ter um diagrama de classe</t>
+  </si>
+  <si>
+    <t>RF01</t>
+  </si>
+  <si>
+    <t>RF02</t>
+  </si>
+  <si>
+    <t>RF03</t>
+  </si>
+  <si>
+    <t>RF04</t>
+  </si>
+  <si>
+    <t>RF05</t>
+  </si>
+  <si>
+    <t>RF06</t>
+  </si>
+  <si>
+    <t>RF07</t>
+  </si>
+  <si>
+    <t>RF08</t>
+  </si>
+  <si>
+    <t>RF09</t>
+  </si>
+  <si>
+    <t>RF10</t>
+  </si>
+  <si>
+    <t>RF11</t>
+  </si>
+  <si>
+    <t>RF12</t>
+  </si>
+  <si>
+    <t>RF13</t>
+  </si>
+  <si>
+    <t>RF14</t>
+  </si>
+  <si>
+    <t>RNF01</t>
+  </si>
+  <si>
+    <t>RNF02</t>
+  </si>
+  <si>
+    <t>RNF03</t>
+  </si>
+  <si>
+    <t>RNF04</t>
+  </si>
+  <si>
+    <t>RNF05</t>
+  </si>
+  <si>
+    <t>RNF06</t>
+  </si>
+  <si>
+    <t>RNF07</t>
+  </si>
+  <si>
+    <t>RNF08</t>
+  </si>
+  <si>
+    <t>RF15</t>
+  </si>
+  <si>
+    <t>O software deve realizar autenticação de login e senha</t>
+  </si>
+  <si>
+    <t>O software deve ter opção de seleção de jogos</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>O software deve mostrar os próximos jogos na tela home</t>
+  </si>
+  <si>
+    <t>RF16</t>
   </si>
 </sst>
 </file>
@@ -376,7 +460,53 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Exo 2"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -387,6 +517,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5756327A-DB72-4400-89F4-782C0049AC31}" name="Tabela1" displayName="Tabela1" ref="A1:I25" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:I25" xr:uid="{55B06B77-CC31-4E93-8CBC-87F7A85E2D4A}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{BFC4269B-E9A2-4751-89B6-EAC0F9FB8536}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{8D0F874A-0382-4DE7-975E-C26834E602AC}" name="Descrição do Requisito"/>
+    <tableColumn id="3" xr3:uid="{C9998A27-EC7E-4EC6-92AA-D9D8A7A1C952}" name="Prioridade"/>
+    <tableColumn id="4" xr3:uid="{A96A790A-7A53-4D5A-9EE9-E841FA450E1B}" name="Tipo Requisito "/>
+    <tableColumn id="5" xr3:uid="{5E75F840-5EB0-4AA9-A0A5-03F5F39781B7}" name="Data da Criação" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{73A1C830-0CCD-4B1F-9D72-0756E68C8983}" name="Data Última Alteração"/>
+    <tableColumn id="7" xr3:uid="{B8F292A9-F3EE-4DFE-81FE-C3C9412399A4}" name="Responsável pela última alteração"/>
+    <tableColumn id="8" xr3:uid="{5D4913E1-07F0-4051-82EC-A4B9D6CA8152}" name="Motivo Última Alteração"/>
+    <tableColumn id="9" xr3:uid="{2EB69F74-7DED-49E5-B9A4-0399398718CF}" name="Situação do Requisito"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,82 +840,82 @@
       <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="19.5" thickBot="1">
+    <row r="1" spans="1:1" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" thickBot="1">
+    <row r="2" spans="1:1" ht="27" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="39" thickBot="1">
+    <row r="3" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="51.75" thickBot="1">
+    <row r="4" spans="1:1" ht="53.4" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="39" thickBot="1">
+    <row r="5" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="39" thickBot="1">
+    <row r="6" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="39" thickBot="1">
+    <row r="7" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="39" thickBot="1">
+    <row r="8" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="39" thickBot="1">
+    <row r="9" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="39" thickBot="1">
+    <row r="10" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="26.25" thickBot="1">
+    <row r="11" spans="1:1" ht="27" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="51.75" thickBot="1">
+    <row r="12" spans="1:1" ht="53.4" thickBot="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="39" thickBot="1">
+    <row r="13" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="39" thickBot="1">
+    <row r="14" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="39" thickBot="1">
+    <row r="15" spans="1:1" ht="40.200000000000003" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -780,26 +928,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD4C22B-F461-46A9-A8F5-D25420A93553}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="78.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="78.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="28.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:11" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -831,6 +979,9 @@
       <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -842,8 +993,11 @@
       </c>
     </row>
     <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -853,39 +1007,51 @@
       </c>
     </row>
     <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -897,6 +1063,9 @@
       </c>
     </row>
     <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -908,19 +1077,25 @@
       </c>
     </row>
     <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -930,6 +1105,9 @@
       </c>
     </row>
     <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -941,6 +1119,9 @@
       </c>
     </row>
     <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -952,58 +1133,68 @@
       </c>
     </row>
     <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="13">
-        <v>43884</v>
-      </c>
-      <c r="G16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" t="s">
-        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -1011,10 +1202,19 @@
       <c r="D17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="E17" s="13">
+        <v>43884</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1022,16 +1222,13 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="13">
-        <v>43886</v>
-      </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1040,15 +1237,18 @@
         <v>29</v>
       </c>
       <c r="E19" s="13">
-        <v>43878</v>
+        <v>43886</v>
       </c>
       <c r="G19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1063,9 +1263,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -1076,10 +1279,16 @@
       <c r="E21" s="13">
         <v>43878</v>
       </c>
-    </row>
-    <row r="22" spans="2:7">
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1090,13 +1299,13 @@
       <c r="E22" s="13">
         <v>43878</v>
       </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -1111,25 +1320,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
       <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="13">
+        <v>43878</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="13">
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="13">
         <v>43891</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>